<commit_message>
crossed dates can be handled
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronnie\Desktop\Python-xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2336B56-AFD6-4D89-A424-D4DA7F9F653A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B761361B-C007-438A-A60F-91469ECE9BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>nome</t>
   </si>
@@ -54,16 +54,19 @@
     <t>005</t>
   </si>
   <si>
-    <t>006</t>
-  </si>
-  <si>
-    <t>007</t>
-  </si>
-  <si>
     <t>pessoa1</t>
   </si>
   <si>
     <t>pessoa2</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
   </si>
 </sst>
 </file>
@@ -73,7 +76,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ \-\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,14 +130,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="2" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Arial Black"/>
@@ -167,7 +162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -186,10 +181,25 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
+        <color theme="5" tint="-0.249977111117893"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
+        <color theme="5" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="5" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="5" tint="-0.249977111117893"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -204,34 +214,6 @@
       <right style="thin">
         <color theme="5" tint="-0.249977111117893"/>
       </right>
-      <top style="thin">
-        <color theme="5" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="5" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="5" tint="-0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color theme="5" tint="-0.249977111117893"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="5" tint="-0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color theme="5" tint="-0.249977111117893"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color theme="5" tint="-0.249977111117893"/>
@@ -296,17 +278,6 @@
         <color theme="5" tint="-0.249977111117893"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top style="thin">
-        <color theme="5" tint="-0.249977111117893"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -325,66 +296,116 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="5" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="5" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="5" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,8 +607,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:D8" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5">
-  <autoFilter ref="A1:D8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5">
+  <autoFilter ref="A1:D9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="nome" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="inicio" dataDxfId="2"/>
@@ -861,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,128 +897,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="16">
-        <v>44734.63082175926</v>
-      </c>
-      <c r="C2" s="9">
-        <v>44734.725949074076</v>
-      </c>
-      <c r="D2" s="21" t="s">
+      <c r="A2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="12">
+        <v>44738.63082175926</v>
+      </c>
+      <c r="C2" s="7">
+        <v>44738.725949074076</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="5">
+      <c r="A3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4">
         <v>44736.416666666664</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>44736.621527777781</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="9">
+      <c r="A4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7">
         <v>44736.479166666664</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>44736.643055555556</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="8">
+      <c r="A5" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6">
         <v>44736.375</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <v>44736.645833333336</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="7">
-        <v>44736.46875</v>
-      </c>
-      <c r="C6" s="7">
-        <v>44736.675000000003</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="20"/>
+      <c r="A6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="19">
+        <v>44736.665277777778</v>
+      </c>
+      <c r="C6" s="20">
+        <v>44736.669768518521</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>11</v>
+      <c r="A7" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="B7" s="5">
-        <v>44740.590277777781</v>
+        <v>44736.46875</v>
       </c>
       <c r="C7" s="5">
-        <v>44740.670138888891</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>9</v>
-      </c>
+        <v>44736.675000000003</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="21">
+        <v>44740.590277777781</v>
+      </c>
+      <c r="C8" s="22">
+        <v>44740.670138888891</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6">
+    </row>
+    <row r="9" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="19">
         <v>44741.665277777778</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C9" s="20">
         <v>44741.669768518521</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-      <c r="C9" s="14"/>
+      <c r="D9" s="17" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="2"/>
+      <c r="F10" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>